<commit_message>
Update template with new options
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/accessioning_template_extended_with_metadata.xlsx
+++ b/docs/public/help/help_linked_docs/accessioning_template_extended_with_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D754EAE-BB66-0B45-AF09-8E5FAB7F8AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03EFCB6-099C-1241-8817-9269125C9748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1620" windowWidth="28800" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
@@ -300,9 +300,6 @@
     <t>Genome Build</t>
   </si>
   <si>
-    <t>hg19, hg38</t>
-  </si>
-  <si>
     <t>Comma-separated</t>
   </si>
   <si>
@@ -318,10 +315,13 @@
     <t>789-3464468</t>
   </si>
   <si>
-    <t>sample_3464468.bam.gz</t>
-  </si>
-  <si>
     <t>Individual ID*</t>
+  </si>
+  <si>
+    <t>hg19, GRCh37, GRCh38</t>
+  </si>
+  <si>
+    <t>sample_3464468.vcf.gz</t>
   </si>
 </sst>
 </file>
@@ -876,30 +876,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23985C4D-01B8-468F-8F7A-3E2DDE3ABF1C}">
   <dimension ref="A1:CB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AN7" sqref="AN7"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AN5" sqref="AN5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1248,7 +1248,7 @@
     <col min="39" max="39" width="14.33203125" style="6" customWidth="1"/>
     <col min="40" max="40" width="42.5" style="5" customWidth="1"/>
     <col min="41" max="41" width="21.1640625" style="8" customWidth="1"/>
-    <col min="42" max="42" width="16" style="8" customWidth="1"/>
+    <col min="42" max="42" width="19.6640625" style="8" customWidth="1"/>
     <col min="43" max="43" width="16" style="61" customWidth="1"/>
     <col min="44" max="76" width="16" style="8" customWidth="1"/>
     <col min="77" max="77" width="14.5" style="5" customWidth="1"/>
@@ -1259,55 +1259,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:80" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="74" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="80" t="s">
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="75"/>
-      <c r="AC1" s="75"/>
-      <c r="AD1" s="75"/>
-      <c r="AE1" s="75"/>
-      <c r="AF1" s="75"/>
-      <c r="AG1" s="75"/>
-      <c r="AH1" s="75"/>
-      <c r="AI1" s="75"/>
-      <c r="AJ1" s="75"/>
-      <c r="AK1" s="75"/>
-      <c r="AL1" s="75"/>
-      <c r="AM1" s="75"/>
-      <c r="AN1" s="75"/>
-      <c r="AO1" s="75"/>
-      <c r="AP1" s="75"/>
-      <c r="AQ1" s="76"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="77"/>
+      <c r="AP1" s="77"/>
+      <c r="AQ1" s="78"/>
       <c r="AR1" s="22"/>
       <c r="AS1" s="22"/>
       <c r="AT1" s="22"/>
@@ -1354,7 +1354,7 @@
         <v>76</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>78</v>
@@ -1474,7 +1474,7 @@
         <v>90</v>
       </c>
       <c r="AQ2" s="69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AR2" s="3"/>
       <c r="AS2" s="3"/>
@@ -1623,13 +1623,13 @@
       </c>
       <c r="AM3" s="57"/>
       <c r="AN3" s="51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AO3" s="72" t="s">
-        <v>92</v>
-      </c>
-      <c r="AP3" s="81" t="s">
         <v>91</v>
+      </c>
+      <c r="AP3" s="74" t="s">
+        <v>97</v>
       </c>
       <c r="AQ3" s="73"/>
       <c r="AR3" s="11"/>
@@ -1761,7 +1761,7 @@
       <c r="AL4" s="45"/>
       <c r="AM4" s="58"/>
       <c r="AN4" s="43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AO4" s="70"/>
       <c r="AP4" s="70"/>
@@ -1855,13 +1855,13 @@
       <c r="AM5" s="59"/>
       <c r="AN5" s="68"/>
       <c r="AO5" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AP5" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AQ5" s="82" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="AQ5" s="75" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:80" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update/add case templates + docs
Also, update compressed VCF file format in inserts to allow submissions.
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/accessioning_template_extended_with_metadata.xlsx
+++ b/docs/public/help/help_linked_docs/accessioning_template_extended_with_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal-2/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7FFDBD-57B2-504E-A4FD-C500019EDC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C030D73-2513-4840-9D25-E17CDE5E3617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1620" windowWidth="28800" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
@@ -231,9 +231,6 @@
     <t>Specimen Type*</t>
   </si>
   <si>
-    <t>Workup Type*</t>
-  </si>
-  <si>
     <t>Research Protocol Name</t>
   </si>
   <si>
@@ -331,6 +328,9 @@
   </si>
   <si>
     <t>SNV</t>
+  </si>
+  <si>
+    <t>Test Requested*</t>
   </si>
 </sst>
 </file>
@@ -850,6 +850,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -870,9 +873,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23985C4D-01B8-468F-8F7A-3E2DDE3ABF1C}">
   <dimension ref="A1:CC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AP6" sqref="AP6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1233,56 +1233,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="64"/>
-      <c r="T1" s="61" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="67" t="s">
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="63"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="62"/>
-      <c r="AK1" s="62"/>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="63"/>
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="63"/>
+      <c r="AJ1" s="63"/>
+      <c r="AK1" s="63"/>
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="64"/>
       <c r="AS1" s="20"/>
       <c r="AT1" s="20"/>
       <c r="AU1" s="20"/>
@@ -1326,19 +1326,19 @@
         <v>65</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>57</v>
@@ -1350,16 +1350,16 @@
         <v>64</v>
       </c>
       <c r="J2" s="47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L2" s="14" t="s">
         <v>40</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>10</v>
@@ -1380,10 +1380,10 @@
         <v>55</v>
       </c>
       <c r="T2" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" s="16" t="s">
         <v>71</v>
-      </c>
-      <c r="U2" s="16" t="s">
-        <v>72</v>
       </c>
       <c r="V2" s="16" t="s">
         <v>13</v>
@@ -1404,13 +1404,13 @@
         <v>67</v>
       </c>
       <c r="AB2" s="18" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="AC2" s="18" t="s">
         <v>22</v>
       </c>
       <c r="AD2" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AE2" s="18" t="s">
         <v>49</v>
@@ -1431,7 +1431,7 @@
         <v>54</v>
       </c>
       <c r="AK2" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AL2" s="18" t="s">
         <v>53</v>
@@ -1440,19 +1440,19 @@
         <v>61</v>
       </c>
       <c r="AN2" s="52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AO2" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP2" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="AP2" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ2" s="68" t="s">
-        <v>99</v>
+      <c r="AQ2" s="61" t="s">
+        <v>98</v>
       </c>
       <c r="AR2" s="54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AS2" s="3"/>
       <c r="AT2" s="3"/>
@@ -1494,16 +1494,16 @@
     </row>
     <row r="3" spans="1:81" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="38" t="s">
+      <c r="D3" s="23" t="s">
         <v>81</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>82</v>
       </c>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
@@ -1511,7 +1511,7 @@
         <v>58</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="23" t="s">
         <v>1</v>
@@ -1567,7 +1567,7 @@
         <v>46</v>
       </c>
       <c r="AB3" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AC3" s="26" t="s">
         <v>0</v>
@@ -1601,16 +1601,16 @@
       </c>
       <c r="AM3" s="42"/>
       <c r="AN3" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AO3" s="57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AP3" s="59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AQ3" s="57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AR3" s="58"/>
       <c r="AS3" s="11"/>
@@ -1652,7 +1652,7 @@
         <v>55432</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="39">
         <v>456</v>
@@ -1742,7 +1742,7 @@
       <c r="AL4" s="31"/>
       <c r="AM4" s="43"/>
       <c r="AN4" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AO4" s="55"/>
       <c r="AP4" s="55"/>
@@ -1754,7 +1754,7 @@
         <v>55432</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="40">
         <v>789</v>
@@ -1836,16 +1836,16 @@
       <c r="AM5" s="44"/>
       <c r="AN5" s="53"/>
       <c r="AO5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AP5" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AQ5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AR5" s="60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:81" ht="15" x14ac:dyDescent="0.2">
@@ -1853,7 +1853,7 @@
         <v>55432</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="38">
         <v>123</v>

</xml_diff>